<commit_message>
excelData and commonsteps changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/excelData.xlsx
+++ b/src/test/resources/testData/excelData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t>username</t>
   </si>
@@ -297,12 +297,18 @@
   <si>
     <t>https://dsportalapp.herokuapp.com/graph/practice</t>
   </si>
+  <si>
+    <t>https://dsportalapp.herokuapp.com/login</t>
+  </si>
+  <si>
+    <t>https://dsportalapp.herokuapp.com/register</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -340,6 +346,11 @@
       <u/>
       <color rgb="FF000000"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -367,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -387,6 +398,9 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -4654,7 +4668,9 @@
       <c r="Z64" s="8"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="8"/>
+      <c r="A65" s="11" t="s">
+        <v>82</v>
+      </c>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
@@ -4710,7 +4726,9 @@
       <c r="Z66" s="8"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="8"/>
+      <c r="A67" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
@@ -11019,7 +11037,9 @@
     <hyperlink r:id="rId53" ref="A61"/>
     <hyperlink r:id="rId54" ref="A62"/>
     <hyperlink r:id="rId55" ref="A63"/>
+    <hyperlink r:id="rId56" ref="A65"/>
+    <hyperlink r:id="rId57" ref="A67"/>
   </hyperlinks>
-  <drawing r:id="rId56"/>
+  <drawing r:id="rId58"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified Excelsheet reader,Login page factory and data structure Intro module
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/excelData.xlsx
+++ b/src/test/resources/testData/excelData.xlsx
@@ -11,14 +11,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="BZyS5d2YIEKcN+BUrRjlCgo3LTg0w6dT9yQIozGRoMc="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="6eA0zEQXE7NLunaWyDe9Es3wmIcezIyEcHzmCS3Up0I="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
   <si>
     <t>username</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>submission success</t>
+  </si>
+  <si>
+    <t>expectedUrls</t>
   </si>
   <si>
     <t>https://dsportalapp.herokuapp.com/</t>
@@ -330,11 +333,11 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <u/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <u/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -378,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -394,6 +397,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
@@ -2796,7 +2802,7 @@
       <c r="Z1" s="8"/>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="8"/>
@@ -2826,7 +2832,9 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -2854,9 +2862,7 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4">
-      <c r="A4" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -2884,7 +2890,9 @@
       <c r="Z4" s="8"/>
     </row>
     <row r="5">
-      <c r="A5" s="8"/>
+      <c r="A5" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -2912,9 +2920,7 @@
       <c r="Z5" s="8"/>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -2942,7 +2948,7 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="8"/>
@@ -2972,7 +2978,7 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="8"/>
@@ -3002,7 +3008,9 @@
       <c r="Z8" s="8"/>
     </row>
     <row r="9">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -3030,9 +3038,7 @@
       <c r="Z9" s="8"/>
     </row>
     <row r="10">
-      <c r="A10" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -3060,7 +3066,7 @@
       <c r="Z10" s="8"/>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="8"/>
@@ -3090,7 +3096,7 @@
       <c r="Z11" s="8"/>
     </row>
     <row r="12">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="8"/>
@@ -3120,7 +3126,7 @@
       <c r="Z12" s="8"/>
     </row>
     <row r="13">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="8"/>
@@ -3150,7 +3156,7 @@
       <c r="Z13" s="8"/>
     </row>
     <row r="14">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="8"/>
@@ -3180,7 +3186,7 @@
       <c r="Z14" s="8"/>
     </row>
     <row r="15">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="10" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="8"/>
@@ -3210,7 +3216,7 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="8"/>
@@ -3240,7 +3246,7 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="10" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="8"/>
@@ -3270,7 +3276,7 @@
       <c r="Z17" s="8"/>
     </row>
     <row r="18">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="10" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="8"/>
@@ -3300,7 +3306,7 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="8"/>
@@ -3330,7 +3336,9 @@
       <c r="Z19" s="8"/>
     </row>
     <row r="20">
-      <c r="A20" s="8"/>
+      <c r="A20" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -3357,10 +3365,8 @@
       <c r="Y20" s="8"/>
       <c r="Z20" s="8"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="9" t="s">
-        <v>43</v>
-      </c>
+    <row r="21">
+      <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -3388,7 +3394,7 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B22" s="8"/>
@@ -3418,7 +3424,7 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B23" s="8"/>
@@ -3448,7 +3454,7 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="8"/>
@@ -3478,7 +3484,7 @@
       <c r="Z24" s="8"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="10" t="s">
         <v>47</v>
       </c>
       <c r="B25" s="8"/>
@@ -3538,7 +3544,7 @@
       <c r="Z26" s="8"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="11" t="s">
         <v>49</v>
       </c>
       <c r="B27" s="8"/>
@@ -3568,7 +3574,7 @@
       <c r="Z27" s="8"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B28" s="8"/>
@@ -3598,7 +3604,7 @@
       <c r="Z28" s="8"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B29" s="8"/>
@@ -3628,7 +3634,9 @@
       <c r="Z29" s="8"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="8"/>
+      <c r="A30" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -3656,9 +3664,7 @@
       <c r="Z30" s="8"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="9" t="s">
-        <v>52</v>
-      </c>
+      <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -3686,7 +3692,7 @@
       <c r="Z31" s="8"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="10" t="s">
         <v>53</v>
       </c>
       <c r="B32" s="8"/>
@@ -3716,7 +3722,7 @@
       <c r="Z32" s="8"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="10" t="s">
         <v>54</v>
       </c>
       <c r="B33" s="8"/>
@@ -3746,7 +3752,7 @@
       <c r="Z33" s="8"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="10" t="s">
         <v>55</v>
       </c>
       <c r="B34" s="8"/>
@@ -3776,7 +3782,7 @@
       <c r="Z34" s="8"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="10" t="s">
         <v>56</v>
       </c>
       <c r="B35" s="8"/>
@@ -3806,7 +3812,9 @@
       <c r="Z35" s="8"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="8"/>
+      <c r="A36" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -3834,9 +3842,7 @@
       <c r="Z36" s="8"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="9" t="s">
-        <v>57</v>
-      </c>
+      <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
@@ -3864,7 +3870,7 @@
       <c r="Z37" s="8"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B38" s="8"/>
@@ -3894,7 +3900,7 @@
       <c r="Z38" s="8"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B39" s="8"/>
@@ -3924,7 +3930,7 @@
       <c r="Z39" s="8"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="10" t="s">
         <v>60</v>
       </c>
       <c r="B40" s="8"/>
@@ -3954,7 +3960,7 @@
       <c r="Z40" s="8"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B41" s="8"/>
@@ -3984,7 +3990,7 @@
       <c r="Z41" s="8"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="10" t="s">
         <v>62</v>
       </c>
       <c r="B42" s="8"/>
@@ -4014,7 +4020,9 @@
       <c r="Z42" s="8"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="8"/>
+      <c r="A43" s="10" t="s">
+        <v>63</v>
+      </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -4042,9 +4050,7 @@
       <c r="Z43" s="8"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -4072,7 +4078,7 @@
       <c r="Z44" s="8"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B45" s="8"/>
@@ -4102,7 +4108,7 @@
       <c r="Z45" s="8"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="10" t="s">
         <v>65</v>
       </c>
       <c r="B46" s="8"/>
@@ -4132,7 +4138,7 @@
       <c r="Z46" s="8"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="10" t="s">
         <v>66</v>
       </c>
       <c r="B47" s="8"/>
@@ -4162,7 +4168,7 @@
       <c r="Z47" s="8"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B48" s="8"/>
@@ -4192,7 +4198,7 @@
       <c r="Z48" s="8"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="10" t="s">
         <v>68</v>
       </c>
       <c r="B49" s="8"/>
@@ -4222,7 +4228,7 @@
       <c r="Z49" s="8"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="10" t="s">
         <v>69</v>
       </c>
       <c r="B50" s="8"/>
@@ -4252,7 +4258,7 @@
       <c r="Z50" s="8"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="10" t="s">
         <v>70</v>
       </c>
       <c r="B51" s="8"/>
@@ -4282,7 +4288,7 @@
       <c r="Z51" s="8"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B52" s="8"/>
@@ -4312,7 +4318,7 @@
       <c r="Z52" s="8"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="10" t="s">
         <v>72</v>
       </c>
       <c r="B53" s="8"/>
@@ -4342,7 +4348,7 @@
       <c r="Z53" s="8"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="10" t="s">
         <v>73</v>
       </c>
       <c r="B54" s="8"/>
@@ -4372,7 +4378,7 @@
       <c r="Z54" s="8"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="10" t="s">
         <v>74</v>
       </c>
       <c r="B55" s="8"/>
@@ -4402,7 +4408,7 @@
       <c r="Z55" s="8"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B56" s="8"/>
@@ -4432,7 +4438,7 @@
       <c r="Z56" s="8"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="9" t="s">
+      <c r="A57" s="10" t="s">
         <v>76</v>
       </c>
       <c r="B57" s="8"/>
@@ -4462,7 +4468,7 @@
       <c r="Z57" s="8"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="10" t="s">
         <v>77</v>
       </c>
       <c r="B58" s="8"/>
@@ -4492,7 +4498,9 @@
       <c r="Z58" s="8"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="8"/>
+      <c r="A59" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
@@ -4520,9 +4528,7 @@
       <c r="Z59" s="8"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="9" t="s">
-        <v>78</v>
-      </c>
+      <c r="A60" s="8"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
@@ -4550,7 +4556,7 @@
       <c r="Z60" s="8"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="9" t="s">
+      <c r="A61" s="10" t="s">
         <v>79</v>
       </c>
       <c r="B61" s="8"/>
@@ -4580,7 +4586,7 @@
       <c r="Z61" s="8"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="10" t="s">
         <v>80</v>
       </c>
       <c r="B62" s="8"/>
@@ -4610,7 +4616,7 @@
       <c r="Z62" s="8"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="10" t="s">
         <v>81</v>
       </c>
       <c r="B63" s="8"/>
@@ -4640,7 +4646,9 @@
       <c r="Z63" s="8"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="8"/>
+      <c r="A64" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
@@ -4668,9 +4676,7 @@
       <c r="Z64" s="8"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="11" t="s">
-        <v>82</v>
-      </c>
+      <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
@@ -4698,7 +4704,9 @@
       <c r="Z65" s="8"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="8"/>
+      <c r="A66" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
@@ -4726,9 +4734,7 @@
       <c r="Z66" s="8"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="11" t="s">
-        <v>83</v>
-      </c>
+      <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
@@ -4756,7 +4762,9 @@
       <c r="Z67" s="8"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="8"/>
+      <c r="A68" s="12" t="s">
+        <v>84</v>
+      </c>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
@@ -10243,7 +10251,34 @@
       <c r="Y263" s="8"/>
       <c r="Z263" s="8"/>
     </row>
-    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1">
+      <c r="A264" s="8"/>
+      <c r="B264" s="8"/>
+      <c r="C264" s="8"/>
+      <c r="D264" s="8"/>
+      <c r="E264" s="8"/>
+      <c r="F264" s="8"/>
+      <c r="G264" s="8"/>
+      <c r="H264" s="8"/>
+      <c r="I264" s="8"/>
+      <c r="J264" s="8"/>
+      <c r="K264" s="8"/>
+      <c r="L264" s="8"/>
+      <c r="M264" s="8"/>
+      <c r="N264" s="8"/>
+      <c r="O264" s="8"/>
+      <c r="P264" s="8"/>
+      <c r="Q264" s="8"/>
+      <c r="R264" s="8"/>
+      <c r="S264" s="8"/>
+      <c r="T264" s="8"/>
+      <c r="U264" s="8"/>
+      <c r="V264" s="8"/>
+      <c r="W264" s="8"/>
+      <c r="X264" s="8"/>
+      <c r="Y264" s="8"/>
+      <c r="Z264" s="8"/>
+    </row>
     <row r="265" ht="15.75" customHeight="1"/>
     <row r="266" ht="15.75" customHeight="1"/>
     <row r="267" ht="15.75" customHeight="1"/>
@@ -10980,65 +11015,66 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A1"/>
-    <hyperlink r:id="rId2" ref="A2"/>
-    <hyperlink r:id="rId3" ref="A4"/>
-    <hyperlink r:id="rId4" ref="A6"/>
-    <hyperlink r:id="rId5" ref="A7"/>
-    <hyperlink r:id="rId6" ref="A8"/>
-    <hyperlink r:id="rId7" ref="A10"/>
-    <hyperlink r:id="rId8" ref="A11"/>
-    <hyperlink r:id="rId9" ref="A12"/>
-    <hyperlink r:id="rId10" ref="A13"/>
-    <hyperlink r:id="rId11" ref="A14"/>
-    <hyperlink r:id="rId12" ref="A15"/>
-    <hyperlink r:id="rId13" ref="A16"/>
-    <hyperlink r:id="rId14" ref="A17"/>
-    <hyperlink r:id="rId15" ref="A18"/>
-    <hyperlink r:id="rId16" ref="A19"/>
-    <hyperlink r:id="rId17" ref="A21"/>
-    <hyperlink r:id="rId18" ref="A22"/>
-    <hyperlink r:id="rId19" ref="A23"/>
-    <hyperlink r:id="rId20" ref="A24"/>
-    <hyperlink r:id="rId21" ref="A25"/>
-    <hyperlink r:id="rId22" ref="A26"/>
-    <hyperlink r:id="rId23" ref="A27"/>
-    <hyperlink r:id="rId24" ref="A28"/>
-    <hyperlink r:id="rId25" ref="A29"/>
-    <hyperlink r:id="rId26" ref="A31"/>
-    <hyperlink r:id="rId27" ref="A32"/>
-    <hyperlink r:id="rId28" ref="A33"/>
-    <hyperlink r:id="rId29" ref="A34"/>
-    <hyperlink r:id="rId30" ref="A35"/>
-    <hyperlink r:id="rId31" ref="A37"/>
-    <hyperlink r:id="rId32" ref="A38"/>
-    <hyperlink r:id="rId33" ref="A39"/>
-    <hyperlink r:id="rId34" ref="A40"/>
-    <hyperlink r:id="rId35" ref="A41"/>
-    <hyperlink r:id="rId36" ref="A42"/>
-    <hyperlink r:id="rId37" ref="A44"/>
-    <hyperlink r:id="rId38" ref="A45"/>
-    <hyperlink r:id="rId39" ref="A46"/>
-    <hyperlink r:id="rId40" ref="A47"/>
-    <hyperlink r:id="rId41" ref="A48"/>
-    <hyperlink r:id="rId42" ref="A49"/>
-    <hyperlink r:id="rId43" ref="A50"/>
-    <hyperlink r:id="rId44" ref="A51"/>
-    <hyperlink r:id="rId45" ref="A52"/>
-    <hyperlink r:id="rId46" ref="A53"/>
-    <hyperlink r:id="rId47" ref="A54"/>
-    <hyperlink r:id="rId48" ref="A55"/>
-    <hyperlink r:id="rId49" ref="A56"/>
-    <hyperlink r:id="rId50" ref="A57"/>
-    <hyperlink r:id="rId51" ref="A58"/>
-    <hyperlink r:id="rId52" ref="A60"/>
-    <hyperlink r:id="rId53" ref="A61"/>
-    <hyperlink r:id="rId54" ref="A62"/>
-    <hyperlink r:id="rId55" ref="A63"/>
-    <hyperlink r:id="rId56" ref="A65"/>
-    <hyperlink r:id="rId57" ref="A67"/>
+    <hyperlink r:id="rId1" ref="A2"/>
+    <hyperlink r:id="rId2" ref="A3"/>
+    <hyperlink r:id="rId3" ref="A5"/>
+    <hyperlink r:id="rId4" ref="A7"/>
+    <hyperlink r:id="rId5" ref="A8"/>
+    <hyperlink r:id="rId6" ref="A9"/>
+    <hyperlink r:id="rId7" ref="A11"/>
+    <hyperlink r:id="rId8" ref="A12"/>
+    <hyperlink r:id="rId9" ref="A13"/>
+    <hyperlink r:id="rId10" ref="A14"/>
+    <hyperlink r:id="rId11" ref="A15"/>
+    <hyperlink r:id="rId12" ref="A16"/>
+    <hyperlink r:id="rId13" ref="A17"/>
+    <hyperlink r:id="rId14" ref="A18"/>
+    <hyperlink r:id="rId15" ref="A19"/>
+    <hyperlink r:id="rId16" ref="A20"/>
+    <hyperlink r:id="rId17" ref="A22"/>
+    <hyperlink r:id="rId18" ref="A23"/>
+    <hyperlink r:id="rId19" ref="A24"/>
+    <hyperlink r:id="rId20" ref="A25"/>
+    <hyperlink r:id="rId21" ref="A26"/>
+    <hyperlink r:id="rId22" ref="A27"/>
+    <hyperlink r:id="rId23" ref="A28"/>
+    <hyperlink r:id="rId24" ref="A29"/>
+    <hyperlink r:id="rId25" ref="A30"/>
+    <hyperlink r:id="rId26" ref="A32"/>
+    <hyperlink r:id="rId27" ref="A33"/>
+    <hyperlink r:id="rId28" ref="A34"/>
+    <hyperlink r:id="rId29" ref="A35"/>
+    <hyperlink r:id="rId30" ref="A36"/>
+    <hyperlink r:id="rId31" ref="A38"/>
+    <hyperlink r:id="rId32" ref="A39"/>
+    <hyperlink r:id="rId33" ref="A40"/>
+    <hyperlink r:id="rId34" ref="A41"/>
+    <hyperlink r:id="rId35" ref="A42"/>
+    <hyperlink r:id="rId36" ref="A43"/>
+    <hyperlink r:id="rId37" ref="A45"/>
+    <hyperlink r:id="rId38" ref="A46"/>
+    <hyperlink r:id="rId39" ref="A47"/>
+    <hyperlink r:id="rId40" ref="A48"/>
+    <hyperlink r:id="rId41" ref="A49"/>
+    <hyperlink r:id="rId42" ref="A50"/>
+    <hyperlink r:id="rId43" ref="A51"/>
+    <hyperlink r:id="rId44" ref="A52"/>
+    <hyperlink r:id="rId45" ref="A53"/>
+    <hyperlink r:id="rId46" ref="A54"/>
+    <hyperlink r:id="rId47" ref="A55"/>
+    <hyperlink r:id="rId48" ref="A56"/>
+    <hyperlink r:id="rId49" ref="A57"/>
+    <hyperlink r:id="rId50" ref="A58"/>
+    <hyperlink r:id="rId51" ref="A59"/>
+    <hyperlink r:id="rId52" ref="A61"/>
+    <hyperlink r:id="rId53" ref="A62"/>
+    <hyperlink r:id="rId54" ref="A63"/>
+    <hyperlink r:id="rId55" ref="A64"/>
+    <hyperlink r:id="rId56" ref="A66"/>
+    <hyperlink r:id="rId57" ref="A68"/>
   </hyperlinks>
   <drawing r:id="rId58"/>
 </worksheet>

</xml_diff>